<commit_message>
Presque fini... Juste couleurs à changer
Reste couleur à changer
</commit_message>
<xml_diff>
--- a/EN - Engine & Powertrain/Cost/EN_A0100.xlsx
+++ b/EN - Engine & Powertrain/Cost/EN_A0100.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="222">
   <si>
     <t>University</t>
   </si>
@@ -897,6 +897,12 @@
   <si>
     <t>Assemble Flat sump + rubber sealing</t>
   </si>
+  <si>
+    <t>Cut (scissors, knife)</t>
+  </si>
+  <si>
+    <t>Sump seal rubber</t>
+  </si>
 </sst>
 </file>
 
@@ -915,7 +921,7 @@
     <numFmt numFmtId="173" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="174" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="175" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;???\ _€_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;???\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -1403,7 +1409,7 @@
     <xf numFmtId="166" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="10" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -1659,7 +1665,8 @@
     <xf numFmtId="1" fontId="23" fillId="0" borderId="2" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="175" fontId="23" fillId="0" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="174" fontId="23" fillId="0" borderId="2" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="23" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -5450,10 +5457,10 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5495,8 +5502,8 @@
         <v>2</v>
       </c>
       <c r="N1" s="102">
-        <f>E12+N19+I32+J42+I46</f>
-        <v>1616.595635972878</v>
+        <f>E12+N19+I33+J43+I47</f>
+        <v>1626.555635972878</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -5539,7 +5546,7 @@
       </c>
       <c r="N4" s="102">
         <f>N1*N2</f>
-        <v>1616.595635972878</v>
+        <v>1626.555635972878</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -5789,7 +5796,7 @@
         <v>2.6634000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="72">
         <v>40</v>
       </c>
@@ -5891,7 +5898,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="83">
-        <f t="shared" ref="I22:I31" si="0">H22*F22*D22</f>
+        <f t="shared" ref="I22:I32" si="0">H22*F22*D22</f>
         <v>0.89400000000000002</v>
       </c>
     </row>
@@ -5925,79 +5932,77 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="72">
+      <c r="A24" s="72"/>
+      <c r="B24" s="72" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="83">
+        <v>0.06</v>
+      </c>
+      <c r="E24" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="138">
+        <v>166</v>
+      </c>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72">
+        <v>1</v>
+      </c>
+      <c r="I24" s="83">
+        <f>F24*H24*D24</f>
+        <v>9.9599999999999991</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="72">
         <v>30</v>
       </c>
-      <c r="B24" s="92" t="s">
+      <c r="B25" s="92" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="89" t="s">
+      <c r="C25" s="89" t="s">
         <v>153</v>
       </c>
-      <c r="D24" s="73">
+      <c r="D25" s="73">
         <v>5.63</v>
       </c>
-      <c r="E24" s="74" t="s">
+      <c r="E25" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="74">
+      <c r="F25" s="74">
         <v>1</v>
       </c>
-      <c r="G24" s="92"/>
-      <c r="H24" s="74">
+      <c r="G25" s="92"/>
+      <c r="H25" s="74">
         <v>1</v>
       </c>
-      <c r="I24" s="83">
+      <c r="I25" s="83">
         <f t="shared" si="0"/>
         <v>5.63</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="72">
-        <v>40</v>
-      </c>
-      <c r="B25" s="92" t="s">
-        <v>152</v>
-      </c>
-      <c r="C25" s="89" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" s="73">
-        <v>0.13</v>
-      </c>
-      <c r="E25" s="90" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="90">
-        <v>1</v>
-      </c>
-      <c r="G25" s="91"/>
-      <c r="H25" s="90">
-        <v>1</v>
-      </c>
-      <c r="I25" s="83">
-        <f t="shared" si="0"/>
-        <v>0.13</v>
-      </c>
-    </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="72">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B26" s="92" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C26" s="89" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D26" s="73">
-        <v>0.75</v>
+        <v>0.13</v>
       </c>
       <c r="E26" s="90" t="s">
         <v>32</v>
       </c>
       <c r="F26" s="90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="91"/>
       <c r="H26" s="90">
@@ -6005,18 +6010,18 @@
       </c>
       <c r="I26" s="83">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="72">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B27" s="92" t="s">
         <v>149</v>
       </c>
       <c r="C27" s="89" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D27" s="73">
         <v>0.75</v>
@@ -6038,16 +6043,16 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="72">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B28" s="92" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C28" s="89" t="s">
         <v>147</v>
       </c>
       <c r="D28" s="73">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="E28" s="90" t="s">
         <v>32</v>
@@ -6061,81 +6066,83 @@
       </c>
       <c r="I28" s="83">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="72">
-        <v>80</v>
-      </c>
-      <c r="B29" s="81" t="s">
-        <v>146</v>
-      </c>
-      <c r="C29" s="81" t="s">
-        <v>219</v>
-      </c>
-      <c r="D29" s="88">
-        <v>0.125</v>
-      </c>
-      <c r="E29" s="87" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="87">
+        <v>70</v>
+      </c>
+      <c r="B29" s="92" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="89" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="73">
+        <v>0.25</v>
+      </c>
+      <c r="E29" s="90" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="90">
         <v>2</v>
       </c>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87">
+      <c r="G29" s="91"/>
+      <c r="H29" s="90">
         <v>1</v>
       </c>
       <c r="I29" s="83">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="72">
-        <v>90</v>
-      </c>
-      <c r="B30" s="124" t="s">
-        <v>145</v>
+        <v>80</v>
+      </c>
+      <c r="B30" s="81" t="s">
+        <v>146</v>
       </c>
       <c r="C30" s="81" t="s">
-        <v>144</v>
-      </c>
-      <c r="D30" s="86">
-        <v>0.5</v>
-      </c>
-      <c r="E30" s="72" t="s">
+        <v>219</v>
+      </c>
+      <c r="D30" s="88">
+        <v>0.125</v>
+      </c>
+      <c r="E30" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="72">
-        <v>12</v>
-      </c>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72">
+      <c r="F30" s="87">
+        <v>2</v>
+      </c>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87">
         <v>1</v>
       </c>
       <c r="I30" s="83">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="72">
-        <v>100</v>
-      </c>
-      <c r="B31" s="81" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" s="81"/>
+        <v>90</v>
+      </c>
+      <c r="B31" s="124" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="81" t="s">
+        <v>144</v>
+      </c>
       <c r="D31" s="86">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="E31" s="72" t="s">
         <v>35</v>
       </c>
       <c r="F31" s="72">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G31" s="72"/>
       <c r="H31" s="72">
@@ -6143,155 +6150,148 @@
       </c>
       <c r="I31" s="83">
         <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="72">
+        <v>100</v>
+      </c>
+      <c r="B32" s="81" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="81"/>
+      <c r="D32" s="86">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="70" t="s">
+      <c r="E32" s="72" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="72">
+        <v>1</v>
+      </c>
+      <c r="G32" s="72"/>
+      <c r="H32" s="72">
+        <v>1</v>
+      </c>
+      <c r="I32" s="83">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="69">
-        <f>SUM(I22:I31)</f>
-        <v>66.417982850000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="76" t="s">
+      <c r="I33" s="69">
+        <f>SUM(I22:I32)</f>
+        <v>76.377982849999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="76" t="s">
+      <c r="B35" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="76" t="s">
+      <c r="C35" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="76" t="s">
+      <c r="D35" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="76" t="s">
+      <c r="E35" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="76" t="s">
+      <c r="F35" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="G34" s="76" t="s">
+      <c r="G35" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="76" t="s">
+      <c r="H35" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="76" t="s">
+      <c r="I35" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="76" t="s">
+      <c r="J35" s="76" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="72">
-        <v>10</v>
-      </c>
-      <c r="B35" s="85" t="s">
-        <v>139</v>
-      </c>
-      <c r="C35" s="72" t="s">
-        <v>142</v>
-      </c>
-      <c r="D35" s="83">
-        <v>1.05</v>
-      </c>
-      <c r="E35" s="72">
-        <v>12</v>
-      </c>
-      <c r="F35" s="82" t="s">
-        <v>30</v>
-      </c>
-      <c r="G35" s="72">
-        <v>80</v>
-      </c>
-      <c r="H35" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="I35" s="80">
-        <v>2</v>
-      </c>
-      <c r="J35" s="73">
-        <f t="shared" ref="J35:J41" si="1">D35*I35</f>
-        <v>2.1</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="72">
-        <v>20</v>
-      </c>
-      <c r="B36" s="84" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="B36" s="85" t="s">
+        <v>139</v>
       </c>
       <c r="C36" s="72" t="s">
         <v>142</v>
       </c>
       <c r="D36" s="83">
-        <v>0.01</v>
-      </c>
-      <c r="E36" s="72"/>
+        <v>1.05</v>
+      </c>
+      <c r="E36" s="72">
+        <v>12</v>
+      </c>
       <c r="F36" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="G36" s="72"/>
-      <c r="H36" s="81"/>
+        <v>30</v>
+      </c>
+      <c r="G36" s="72">
+        <v>80</v>
+      </c>
+      <c r="H36" s="81" t="s">
+        <v>30</v>
+      </c>
       <c r="I36" s="80">
         <v>2</v>
       </c>
       <c r="J36" s="73">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
+        <f t="shared" ref="J36:J42" si="1">D36*I36</f>
+        <v>2.1</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="72">
         <v>20</v>
       </c>
-      <c r="B37" s="85" t="s">
-        <v>139</v>
+      <c r="B37" s="84" t="s">
+        <v>37</v>
       </c>
       <c r="C37" s="72" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D37" s="83">
-        <v>1.4</v>
-      </c>
-      <c r="E37" s="72">
-        <v>12</v>
-      </c>
+        <v>0.01</v>
+      </c>
+      <c r="E37" s="72"/>
       <c r="F37" s="82" t="s">
-        <v>30</v>
-      </c>
-      <c r="G37" s="72">
-        <v>100</v>
-      </c>
-      <c r="H37" s="81" t="s">
-        <v>30</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G37" s="72"/>
+      <c r="H37" s="81"/>
       <c r="I37" s="80">
         <v>2</v>
       </c>
       <c r="J37" s="73">
         <f t="shared" si="1"/>
-        <v>2.8</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="72">
-        <v>30</v>
-      </c>
-      <c r="B38" s="84" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="B38" s="85" t="s">
+        <v>139</v>
       </c>
       <c r="C38" s="72" t="s">
         <v>141</v>
       </c>
       <c r="D38" s="83">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
       <c r="E38" s="72">
         <v>12</v>
@@ -6299,210 +6299,243 @@
       <c r="F38" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="72"/>
-      <c r="H38" s="81"/>
+      <c r="G38" s="72">
+        <v>100</v>
+      </c>
+      <c r="H38" s="81" t="s">
+        <v>30</v>
+      </c>
       <c r="I38" s="80">
         <v>2</v>
       </c>
       <c r="J38" s="73">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="72">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B39" s="84" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39" s="72" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D39" s="83">
-        <v>0.01</v>
-      </c>
-      <c r="E39" s="72"/>
+        <v>0.1</v>
+      </c>
+      <c r="E39" s="72">
+        <v>12</v>
+      </c>
       <c r="F39" s="82" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G39" s="72"/>
       <c r="H39" s="81"/>
       <c r="I39" s="80">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J39" s="73">
         <f t="shared" si="1"/>
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="72">
-        <v>50</v>
-      </c>
-      <c r="B40" s="85" t="s">
-        <v>139</v>
+        <v>40</v>
+      </c>
+      <c r="B40" s="84" t="s">
+        <v>37</v>
       </c>
       <c r="C40" s="72" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D40" s="83">
-        <f>0.8/105154*E40^2*G40*SQRT(G40)+(0.003*EXP(0.319*E40))</f>
-        <v>3.6251689343322346E-2</v>
-      </c>
-      <c r="E40" s="72">
+        <v>0.01</v>
+      </c>
+      <c r="E40" s="72"/>
+      <c r="F40" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="G40" s="72"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="80">
         <v>6</v>
-      </c>
-      <c r="F40" s="82" t="s">
-        <v>30</v>
-      </c>
-      <c r="G40" s="72">
-        <v>15</v>
-      </c>
-      <c r="H40" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="80">
-        <v>12</v>
       </c>
       <c r="J40" s="73">
         <f t="shared" si="1"/>
-        <v>0.43502027211986816</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="72">
-        <v>40</v>
-      </c>
-      <c r="B41" s="84" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="B41" s="85" t="s">
+        <v>139</v>
       </c>
       <c r="C41" s="72" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D41" s="83">
-        <v>0.01</v>
-      </c>
-      <c r="E41" s="72"/>
+        <f>0.8/105154*E41^2*G41*SQRT(G41)+(0.003*EXP(0.319*E41))</f>
+        <v>3.6251689343322346E-2</v>
+      </c>
+      <c r="E41" s="72">
+        <v>6</v>
+      </c>
       <c r="F41" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="G41" s="72"/>
-      <c r="H41" s="81"/>
+        <v>30</v>
+      </c>
+      <c r="G41" s="72">
+        <v>15</v>
+      </c>
+      <c r="H41" s="81" t="s">
+        <v>30</v>
+      </c>
       <c r="I41" s="80">
         <v>12</v>
       </c>
       <c r="J41" s="73">
         <f t="shared" si="1"/>
+        <v>0.43502027211986816</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="72">
+        <v>40</v>
+      </c>
+      <c r="B42" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="72" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" s="83">
+        <v>0.01</v>
+      </c>
+      <c r="E42" s="72"/>
+      <c r="F42" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="72"/>
+      <c r="H42" s="81"/>
+      <c r="I42" s="80">
+        <v>12</v>
+      </c>
+      <c r="J42" s="73">
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="68"/>
-      <c r="B42" s="68"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="70" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="68"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="79">
-        <f>SUM(J35:J41)</f>
+      <c r="J43" s="79">
+        <f>SUM(J36:J42)</f>
         <v>5.7350202721198675</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="67"/>
-      <c r="B43" s="67"/>
-      <c r="C43" s="67"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="67"/>
-      <c r="G43" s="67"/>
-      <c r="H43" s="78"/>
-      <c r="I43" s="77"/>
-      <c r="J43" s="67"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="76" t="s">
+    <row r="44" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="67"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="78"/>
+      <c r="I44" s="77"/>
+      <c r="J44" s="67"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="76" t="s">
+      <c r="B45" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="76" t="s">
+      <c r="C45" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="76" t="s">
+      <c r="D45" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="76" t="s">
+      <c r="E45" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="F44" s="76" t="s">
+      <c r="F45" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="G44" s="76" t="s">
+      <c r="G45" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="H44" s="76" t="s">
+      <c r="H45" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="I44" s="76" t="s">
+      <c r="I45" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="J44" s="68"/>
-    </row>
-    <row r="45" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="72">
+      <c r="J45" s="68"/>
+    </row>
+    <row r="46" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="72">
         <v>10</v>
       </c>
-      <c r="B45" s="75" t="s">
+      <c r="B46" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="74" t="s">
+      <c r="C46" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="73">
+      <c r="D46" s="73">
         <v>500</v>
       </c>
-      <c r="E45" s="72" t="s">
+      <c r="E46" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="72">
+      <c r="F46" s="72">
         <v>4</v>
       </c>
-      <c r="G45" s="72">
+      <c r="G46" s="72">
         <v>3000</v>
       </c>
-      <c r="H45" s="72">
+      <c r="H46" s="72">
         <v>1</v>
       </c>
-      <c r="I45" s="71">
-        <f>D45*F45/G45*H45</f>
+      <c r="I46" s="71">
+        <f>D46*F46/G46*H46</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J45" s="67"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="68"/>
-      <c r="B46" s="68"/>
-      <c r="C46" s="68"/>
-      <c r="D46" s="68"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="68"/>
-      <c r="G46" s="68"/>
-      <c r="H46" s="70" t="s">
+      <c r="J46" s="67"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="68"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="68"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="I46" s="69">
-        <f>SUM(I45:I45)</f>
+      <c r="I47" s="69">
+        <f>SUM(I46:I46)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J46" s="68"/>
+      <c r="J47" s="68"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6530,7 +6563,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="49" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fin cost EN_A001, EN_A005 et EN_A006
Modif couleurs pour coller au template
</commit_message>
<xml_diff>
--- a/EN - Engine & Powertrain/Cost/EN_A0100.xlsx
+++ b/EN - Engine & Powertrain/Cost/EN_A0100.xlsx
@@ -10,7 +10,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8196" activeTab="2"/>
+    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8196" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -1163,13 +1163,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFC4D79B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
+        <fgColor rgb="FFD8E4BC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1560,21 +1560,15 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="24" fillId="9" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="10" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="9" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="39" fontId="23" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1606,7 +1600,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="14" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1616,31 +1609,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="14" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="24" fillId="10" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="24" fillId="10" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="24" fillId="10" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="23" fillId="0" borderId="2" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="23" fillId="0" borderId="2" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="23" fillId="0" borderId="2" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="15" xfId="14" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="14"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
@@ -1667,6 +1648,25 @@
     <xf numFmtId="174" fontId="23" fillId="0" borderId="2" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="23" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="23" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="24" fillId="9" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="9" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="24" fillId="10" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="24" fillId="10" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="24" fillId="10" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="15" xfId="14" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -1755,6 +1755,9 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFD8E4BC"/>
+      <color rgb="FFC4D79B"/>
+      <color rgb="FF76933C"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FF66CCFF"/>
       <color rgb="FF33CCFF"/>
@@ -5454,13 +5457,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FF92D050"/>
+    <tabColor rgb="FF76933C"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5483,85 +5486,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="126" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="101" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="101" t="s">
+      <c r="J1" s="126" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="105">
+      <c r="K1" s="100">
         <v>81</v>
       </c>
-      <c r="M1" s="101" t="s">
+      <c r="M1" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="102">
+      <c r="N1" s="97">
         <f>E12+N19+I33+J43+I47</f>
         <v>1626.555635972878</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="126" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="67" t="s">
         <v>172</v>
       </c>
-      <c r="M2" s="101" t="s">
+      <c r="M2" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="104">
+      <c r="N2" s="99">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="126" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="67" t="s">
         <v>171</v>
       </c>
-      <c r="J3" s="101" t="s">
+      <c r="J3" s="126" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="98" t="s">
         <v>131</v>
       </c>
-      <c r="J4" s="101" t="s">
+      <c r="J4" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="101" t="s">
+      <c r="M4" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="102">
+      <c r="N4" s="97">
         <f>N1*N2</f>
         <v>1626.555635972878</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="126" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="101" t="s">
+      <c r="J5" s="126" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="101" t="s">
+      <c r="A6" s="126" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="67" t="s">
@@ -5569,863 +5572,863 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="127" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="72">
+      <c r="A9" s="70">
         <v>10</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="B9" s="96" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="73">
+      <c r="C9" s="71">
         <f>'EN 01001'!N1</f>
         <v>38.781627930666666</v>
       </c>
-      <c r="D9" s="81">
+      <c r="D9" s="77">
         <v>1</v>
       </c>
-      <c r="E9" s="71">
+      <c r="E9" s="69">
         <f>C9*D9</f>
         <v>38.781627930666666</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="72">
+      <c r="A10" s="70">
         <v>20</v>
       </c>
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="96" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="73">
+      <c r="C10" s="71">
         <f>'EN 01002'!N1</f>
         <v>1.4174720000000001</v>
       </c>
-      <c r="D10" s="81">
+      <c r="D10" s="77">
         <v>2</v>
       </c>
-      <c r="E10" s="71">
+      <c r="E10" s="69">
         <f>C10*D10</f>
         <v>2.8349440000000001</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="72">
+      <c r="A11" s="70">
         <v>30</v>
       </c>
-      <c r="B11" s="100" t="s">
+      <c r="B11" s="96" t="s">
         <v>167</v>
       </c>
-      <c r="C11" s="73">
+      <c r="C11" s="71">
         <f>'EN 01003'!N1</f>
         <v>1.9460502534247164</v>
       </c>
-      <c r="D11" s="81">
+      <c r="D11" s="77">
         <v>1</v>
       </c>
-      <c r="E11" s="71">
+      <c r="E11" s="69">
         <f>C11*D11</f>
         <v>1.9460502534247164</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="79">
+      <c r="E12" s="128">
         <f>SUM(E9:E11)</f>
         <v>43.562622184091381</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="76" t="s">
+      <c r="B14" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="76" t="s">
+      <c r="C14" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="76" t="s">
+      <c r="D14" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="76" t="s">
+      <c r="E14" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="76" t="s">
+      <c r="F14" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="76" t="s">
+      <c r="G14" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="76" t="s">
+      <c r="H14" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="76" t="s">
+      <c r="I14" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="76" t="s">
+      <c r="J14" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="76" t="s">
+      <c r="K14" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="76" t="s">
+      <c r="L14" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="M14" s="76" t="s">
+      <c r="M14" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="76" t="s">
+      <c r="N14" s="127" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="72">
+      <c r="A15" s="70">
         <v>10</v>
       </c>
-      <c r="B15" s="99" t="s">
+      <c r="B15" s="95" t="s">
         <v>166</v>
       </c>
-      <c r="C15" s="72" t="s">
+      <c r="C15" s="70" t="s">
         <v>165</v>
       </c>
-      <c r="D15" s="73">
+      <c r="D15" s="71">
         <v>2.5</v>
       </c>
-      <c r="E15" s="72">
+      <c r="E15" s="70">
         <v>599</v>
       </c>
-      <c r="F15" s="72" t="s">
+      <c r="F15" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72">
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="70">
         <v>1</v>
       </c>
-      <c r="N15" s="98">
+      <c r="N15" s="94">
         <f>E15*D15*M15</f>
         <v>1497.5</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="72">
+      <c r="A16" s="70">
         <v>20</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="70" t="s">
         <v>163</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="73">
+      <c r="D16" s="71">
         <v>0.75</v>
       </c>
-      <c r="E16" s="72">
+      <c r="E16" s="70">
         <v>3.5</v>
       </c>
-      <c r="F16" s="72" t="s">
+      <c r="F16" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="G16" s="72"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="96"/>
-      <c r="K16" s="95"/>
-      <c r="L16" s="95"/>
-      <c r="M16" s="94">
+      <c r="G16" s="70"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="91"/>
+      <c r="M16" s="90">
         <v>3.5</v>
       </c>
-      <c r="N16" s="71">
+      <c r="N16" s="69">
         <f>IF(J16="",D16*M16,D16*J16*K16*L16*M16)</f>
         <v>2.625</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="72">
+      <c r="A17" s="70">
         <v>30</v>
       </c>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="73">
+      <c r="D17" s="71">
         <v>10</v>
       </c>
-      <c r="E17" s="93">
+      <c r="E17" s="89">
         <f>26.634/10000</f>
         <v>2.6634000000000002E-3</v>
       </c>
-      <c r="F17" s="72" t="s">
+      <c r="F17" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="G17" s="72"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="95"/>
-      <c r="M17" s="93">
+      <c r="G17" s="70"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="91"/>
+      <c r="L17" s="91"/>
+      <c r="M17" s="89">
         <f>26.634/10000</f>
         <v>2.6634000000000002E-3</v>
       </c>
-      <c r="N17" s="71">
+      <c r="N17" s="69">
         <f>IF(J17="",D17*M17,D17*J17*K17*L17*M17)</f>
         <v>2.6634000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="72">
+      <c r="A18" s="70">
         <v>40</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="70" t="s">
         <v>217</v>
       </c>
-      <c r="C18" s="119" t="s">
+      <c r="C18" s="107" t="s">
         <v>218</v>
       </c>
-      <c r="D18" s="73">
+      <c r="D18" s="71">
         <v>3.3</v>
       </c>
-      <c r="E18" s="137">
+      <c r="E18" s="124">
         <f>L18*K18*J18</f>
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="70" t="s">
         <v>192</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="95"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="136">
+      <c r="G18" s="70"/>
+      <c r="H18" s="91"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="123">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="K18" s="136">
+      <c r="K18" s="123">
         <v>1E-3</v>
       </c>
-      <c r="L18" s="96">
+      <c r="L18" s="92">
         <v>1100</v>
       </c>
-      <c r="M18" s="94">
+      <c r="M18" s="90">
         <v>1</v>
       </c>
-      <c r="N18" s="71">
+      <c r="N18" s="69">
         <f>M18*E18*D18</f>
         <v>6.1710000000000001E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="M19" s="70" t="s">
+      <c r="M19" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="N19" s="79">
+      <c r="N19" s="128">
         <f>SUM(N15:N18)</f>
         <v>1500.213344</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="76" t="s">
+      <c r="A21" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="127" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="76" t="s">
+      <c r="C21" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="76" t="s">
+      <c r="D21" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="76" t="s">
+      <c r="E21" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="76" t="s">
+      <c r="F21" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="76" t="s">
+      <c r="G21" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="76" t="s">
+      <c r="H21" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="I21" s="76" t="s">
+      <c r="I21" s="127" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="72">
+      <c r="A22" s="70">
         <v>10</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="70" t="s">
         <v>158</v>
       </c>
-      <c r="D22" s="83">
+      <c r="D22" s="79">
         <v>0.15</v>
       </c>
-      <c r="E22" s="72" t="s">
+      <c r="E22" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="70">
         <v>5.96</v>
       </c>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72">
+      <c r="G22" s="70"/>
+      <c r="H22" s="70">
         <v>1</v>
       </c>
-      <c r="I22" s="83">
+      <c r="I22" s="79">
         <f t="shared" ref="I22:I32" si="0">H22*F22*D22</f>
         <v>0.89400000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="72">
+      <c r="A23" s="70">
         <v>20</v>
       </c>
-      <c r="B23" s="72" t="s">
+      <c r="B23" s="70" t="s">
         <v>157</v>
       </c>
-      <c r="C23" s="72" t="s">
+      <c r="C23" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="D23" s="83">
+      <c r="D23" s="79">
         <v>5.25</v>
       </c>
-      <c r="E23" s="72" t="s">
+      <c r="E23" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="F23" s="93">
+      <c r="F23" s="89">
         <f>26.634/10000</f>
         <v>2.6634000000000002E-3</v>
       </c>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72">
+      <c r="G23" s="70"/>
+      <c r="H23" s="70">
         <v>1</v>
       </c>
-      <c r="I23" s="83">
+      <c r="I23" s="79">
         <f t="shared" si="0"/>
         <v>1.3982850000000002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="72"/>
-      <c r="B24" s="72" t="s">
+      <c r="A24" s="70"/>
+      <c r="B24" s="70" t="s">
         <v>220</v>
       </c>
-      <c r="C24" s="72" t="s">
+      <c r="C24" s="70" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="83">
+      <c r="D24" s="79">
         <v>0.06</v>
       </c>
-      <c r="E24" s="72" t="s">
+      <c r="E24" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="138">
+      <c r="F24" s="125">
         <v>166</v>
       </c>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72">
+      <c r="G24" s="70"/>
+      <c r="H24" s="70">
         <v>1</v>
       </c>
-      <c r="I24" s="83">
+      <c r="I24" s="79">
         <f>F24*H24*D24</f>
         <v>9.9599999999999991</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="72">
+      <c r="A25" s="70">
         <v>30</v>
       </c>
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="88" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="89" t="s">
+      <c r="C25" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="D25" s="73">
+      <c r="D25" s="71">
         <v>5.63</v>
       </c>
-      <c r="E25" s="74" t="s">
+      <c r="E25" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="74">
+      <c r="F25" s="72">
         <v>1</v>
       </c>
-      <c r="G25" s="92"/>
-      <c r="H25" s="74">
+      <c r="G25" s="88"/>
+      <c r="H25" s="72">
         <v>1</v>
       </c>
-      <c r="I25" s="83">
+      <c r="I25" s="79">
         <f t="shared" si="0"/>
         <v>5.63</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="72">
+      <c r="A26" s="70">
         <v>40</v>
       </c>
-      <c r="B26" s="92" t="s">
+      <c r="B26" s="88" t="s">
         <v>152</v>
       </c>
-      <c r="C26" s="89" t="s">
+      <c r="C26" s="85" t="s">
         <v>151</v>
       </c>
-      <c r="D26" s="73">
+      <c r="D26" s="71">
         <v>0.13</v>
       </c>
-      <c r="E26" s="90" t="s">
+      <c r="E26" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="90">
+      <c r="F26" s="86">
         <v>1</v>
       </c>
-      <c r="G26" s="91"/>
-      <c r="H26" s="90">
+      <c r="G26" s="87"/>
+      <c r="H26" s="86">
         <v>1</v>
       </c>
-      <c r="I26" s="83">
+      <c r="I26" s="79">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="72">
+      <c r="A27" s="70">
         <v>50</v>
       </c>
-      <c r="B27" s="92" t="s">
+      <c r="B27" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="D27" s="73">
+      <c r="D27" s="71">
         <v>0.75</v>
       </c>
-      <c r="E27" s="90" t="s">
+      <c r="E27" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="90">
+      <c r="F27" s="86">
         <v>2</v>
       </c>
-      <c r="G27" s="91"/>
-      <c r="H27" s="90">
+      <c r="G27" s="87"/>
+      <c r="H27" s="86">
         <v>1</v>
       </c>
-      <c r="I27" s="83">
+      <c r="I27" s="79">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="72">
+      <c r="A28" s="70">
         <v>60</v>
       </c>
-      <c r="B28" s="92" t="s">
+      <c r="B28" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="89" t="s">
+      <c r="C28" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="D28" s="73">
+      <c r="D28" s="71">
         <v>0.75</v>
       </c>
-      <c r="E28" s="90" t="s">
+      <c r="E28" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="90">
+      <c r="F28" s="86">
         <v>2</v>
       </c>
-      <c r="G28" s="91"/>
-      <c r="H28" s="90">
+      <c r="G28" s="87"/>
+      <c r="H28" s="86">
         <v>1</v>
       </c>
-      <c r="I28" s="83">
+      <c r="I28" s="79">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="72">
+      <c r="A29" s="70">
         <v>70</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B29" s="88" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="89" t="s">
+      <c r="C29" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="73">
+      <c r="D29" s="71">
         <v>0.25</v>
       </c>
-      <c r="E29" s="90" t="s">
+      <c r="E29" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="90">
+      <c r="F29" s="86">
         <v>2</v>
       </c>
-      <c r="G29" s="91"/>
-      <c r="H29" s="90">
+      <c r="G29" s="87"/>
+      <c r="H29" s="86">
         <v>1</v>
       </c>
-      <c r="I29" s="83">
+      <c r="I29" s="79">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="72">
+      <c r="A30" s="70">
         <v>80</v>
       </c>
-      <c r="B30" s="81" t="s">
+      <c r="B30" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="C30" s="81" t="s">
+      <c r="C30" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="D30" s="88">
+      <c r="D30" s="84">
         <v>0.125</v>
       </c>
-      <c r="E30" s="87" t="s">
+      <c r="E30" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="87">
+      <c r="F30" s="83">
         <v>2</v>
       </c>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87">
+      <c r="G30" s="83"/>
+      <c r="H30" s="83">
         <v>1</v>
       </c>
-      <c r="I30" s="83">
+      <c r="I30" s="79">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="72">
+      <c r="A31" s="70">
         <v>90</v>
       </c>
-      <c r="B31" s="124" t="s">
+      <c r="B31" s="111" t="s">
         <v>145</v>
       </c>
-      <c r="C31" s="81" t="s">
+      <c r="C31" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="86">
+      <c r="D31" s="82">
         <v>0.5</v>
       </c>
-      <c r="E31" s="72" t="s">
+      <c r="E31" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="72">
+      <c r="F31" s="70">
         <v>12</v>
       </c>
-      <c r="G31" s="72"/>
-      <c r="H31" s="72">
+      <c r="G31" s="70"/>
+      <c r="H31" s="70">
         <v>1</v>
       </c>
-      <c r="I31" s="83">
+      <c r="I31" s="79">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="72">
+      <c r="A32" s="70">
         <v>100</v>
       </c>
-      <c r="B32" s="81" t="s">
+      <c r="B32" s="77" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="81"/>
-      <c r="D32" s="86">
+      <c r="C32" s="77"/>
+      <c r="D32" s="82">
         <v>50</v>
       </c>
-      <c r="E32" s="72" t="s">
+      <c r="E32" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="72">
+      <c r="F32" s="70">
         <v>1</v>
       </c>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72">
+      <c r="G32" s="70"/>
+      <c r="H32" s="70">
         <v>1</v>
       </c>
-      <c r="I32" s="83">
+      <c r="I32" s="79">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H33" s="70" t="s">
+      <c r="H33" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="I33" s="69">
+      <c r="I33" s="130">
         <f>SUM(I22:I32)</f>
         <v>76.377982849999995</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="76" t="s">
+      <c r="A35" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="76" t="s">
+      <c r="B35" s="127" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="76" t="s">
+      <c r="C35" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="76" t="s">
+      <c r="D35" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="76" t="s">
+      <c r="E35" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="76" t="s">
+      <c r="F35" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="G35" s="76" t="s">
+      <c r="G35" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="76" t="s">
+      <c r="H35" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="I35" s="76" t="s">
+      <c r="I35" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="76" t="s">
+      <c r="J35" s="127" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="72">
+      <c r="A36" s="70">
         <v>10</v>
       </c>
-      <c r="B36" s="85" t="s">
+      <c r="B36" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="C36" s="72" t="s">
+      <c r="C36" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="D36" s="83">
+      <c r="D36" s="79">
         <v>1.05</v>
       </c>
-      <c r="E36" s="72">
+      <c r="E36" s="70">
         <v>12</v>
       </c>
-      <c r="F36" s="82" t="s">
+      <c r="F36" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="G36" s="72">
+      <c r="G36" s="70">
         <v>80</v>
       </c>
-      <c r="H36" s="81" t="s">
+      <c r="H36" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="80">
+      <c r="I36" s="76">
         <v>2</v>
       </c>
-      <c r="J36" s="73">
+      <c r="J36" s="71">
         <f t="shared" ref="J36:J42" si="1">D36*I36</f>
         <v>2.1</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="72">
+      <c r="A37" s="70">
         <v>20</v>
       </c>
-      <c r="B37" s="84" t="s">
+      <c r="B37" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="72" t="s">
+      <c r="C37" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="83">
+      <c r="D37" s="79">
         <v>0.01</v>
       </c>
-      <c r="E37" s="72"/>
-      <c r="F37" s="82" t="s">
+      <c r="E37" s="70"/>
+      <c r="F37" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="72"/>
-      <c r="H37" s="81"/>
-      <c r="I37" s="80">
+      <c r="G37" s="70"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="76">
         <v>2</v>
       </c>
-      <c r="J37" s="73">
+      <c r="J37" s="71">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="72">
+      <c r="A38" s="70">
         <v>20</v>
       </c>
-      <c r="B38" s="85" t="s">
+      <c r="B38" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="C38" s="72" t="s">
+      <c r="C38" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D38" s="83">
+      <c r="D38" s="79">
         <v>1.4</v>
       </c>
-      <c r="E38" s="72">
+      <c r="E38" s="70">
         <v>12</v>
       </c>
-      <c r="F38" s="82" t="s">
+      <c r="F38" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="72">
+      <c r="G38" s="70">
         <v>100</v>
       </c>
-      <c r="H38" s="81" t="s">
+      <c r="H38" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="I38" s="80">
+      <c r="I38" s="76">
         <v>2</v>
       </c>
-      <c r="J38" s="73">
+      <c r="J38" s="71">
         <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="72">
+      <c r="A39" s="70">
         <v>30</v>
       </c>
-      <c r="B39" s="84" t="s">
+      <c r="B39" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="72" t="s">
+      <c r="C39" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="D39" s="83">
+      <c r="D39" s="79">
         <v>0.1</v>
       </c>
-      <c r="E39" s="72">
+      <c r="E39" s="70">
         <v>12</v>
       </c>
-      <c r="F39" s="82" t="s">
+      <c r="F39" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="72"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="80">
+      <c r="G39" s="70"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="76">
         <v>2</v>
       </c>
-      <c r="J39" s="73">
+      <c r="J39" s="71">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="72">
+      <c r="A40" s="70">
         <v>40</v>
       </c>
-      <c r="B40" s="84" t="s">
+      <c r="B40" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="72" t="s">
+      <c r="C40" s="70" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="83">
+      <c r="D40" s="79">
         <v>0.01</v>
       </c>
-      <c r="E40" s="72"/>
-      <c r="F40" s="82" t="s">
+      <c r="E40" s="70"/>
+      <c r="F40" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="G40" s="72"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="80">
+      <c r="G40" s="70"/>
+      <c r="H40" s="77"/>
+      <c r="I40" s="76">
         <v>6</v>
       </c>
-      <c r="J40" s="73">
+      <c r="J40" s="71">
         <f t="shared" si="1"/>
         <v>0.06</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="72">
+      <c r="A41" s="70">
         <v>50</v>
       </c>
-      <c r="B41" s="85" t="s">
+      <c r="B41" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="72" t="s">
+      <c r="C41" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="83">
+      <c r="D41" s="79">
         <f>0.8/105154*E41^2*G41*SQRT(G41)+(0.003*EXP(0.319*E41))</f>
         <v>3.6251689343322346E-2</v>
       </c>
-      <c r="E41" s="72">
+      <c r="E41" s="70">
         <v>6</v>
       </c>
-      <c r="F41" s="82" t="s">
+      <c r="F41" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="72">
+      <c r="G41" s="70">
         <v>15</v>
       </c>
-      <c r="H41" s="81" t="s">
+      <c r="H41" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="I41" s="80">
+      <c r="I41" s="76">
         <v>12</v>
       </c>
-      <c r="J41" s="73">
+      <c r="J41" s="71">
         <f t="shared" si="1"/>
         <v>0.43502027211986816</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="72">
+      <c r="A42" s="70">
         <v>40</v>
       </c>
-      <c r="B42" s="84" t="s">
+      <c r="B42" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="70" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="83">
+      <c r="D42" s="79">
         <v>0.01</v>
       </c>
-      <c r="E42" s="72"/>
-      <c r="F42" s="82" t="s">
+      <c r="E42" s="70"/>
+      <c r="F42" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="72"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="80">
+      <c r="G42" s="70"/>
+      <c r="H42" s="77"/>
+      <c r="I42" s="76">
         <v>12</v>
       </c>
-      <c r="J42" s="73">
+      <c r="J42" s="71">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
@@ -6439,10 +6442,10 @@
       <c r="F43" s="68"/>
       <c r="G43" s="68"/>
       <c r="H43" s="68"/>
-      <c r="I43" s="70" t="s">
+      <c r="I43" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="J43" s="79">
+      <c r="J43" s="128">
         <f>SUM(J36:J42)</f>
         <v>5.7350202721198675</v>
       </c>
@@ -6455,66 +6458,66 @@
       <c r="E44" s="67"/>
       <c r="F44" s="67"/>
       <c r="G44" s="67"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="77"/>
+      <c r="H44" s="75"/>
+      <c r="I44" s="74"/>
       <c r="J44" s="67"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="76" t="s">
+      <c r="A45" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="76" t="s">
+      <c r="B45" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="76" t="s">
+      <c r="C45" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="76" t="s">
+      <c r="D45" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="76" t="s">
+      <c r="E45" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="76" t="s">
+      <c r="F45" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="G45" s="76" t="s">
+      <c r="G45" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="H45" s="76" t="s">
+      <c r="H45" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="I45" s="76" t="s">
+      <c r="I45" s="127" t="s">
         <v>18</v>
       </c>
       <c r="J45" s="68"/>
     </row>
     <row r="46" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="72">
+      <c r="A46" s="70">
         <v>10</v>
       </c>
-      <c r="B46" s="75" t="s">
+      <c r="B46" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="74" t="s">
+      <c r="C46" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="D46" s="73">
+      <c r="D46" s="71">
         <v>500</v>
       </c>
-      <c r="E46" s="72" t="s">
+      <c r="E46" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="F46" s="72">
+      <c r="F46" s="70">
         <v>4</v>
       </c>
-      <c r="G46" s="72">
+      <c r="G46" s="70">
         <v>3000</v>
       </c>
-      <c r="H46" s="72">
+      <c r="H46" s="70">
         <v>1</v>
       </c>
-      <c r="I46" s="71">
+      <c r="I46" s="69">
         <f>D46*F46/G46*H46</f>
         <v>0.66666666666666663</v>
       </c>
@@ -6528,10 +6531,10 @@
       <c r="E47" s="68"/>
       <c r="F47" s="68"/>
       <c r="G47" s="68"/>
-      <c r="H47" s="70" t="s">
+      <c r="H47" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="I47" s="69">
+      <c r="I47" s="130">
         <f>SUM(I46:I46)</f>
         <v>0.66666666666666663</v>
       </c>
@@ -6557,13 +6560,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFCCFFCC"/>
+    <tabColor rgb="FFC4D79B"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="49" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6596,95 +6599,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="101" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="118" t="s">
+      <c r="J1" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="105">
+      <c r="K1" s="100">
         <v>81</v>
       </c>
-      <c r="M1" s="116" t="s">
+      <c r="M1" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="102">
+      <c r="N1" s="97">
         <f>N15+I30+I34</f>
         <v>38.781627930666666</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="131" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="67" t="s">
         <v>172</v>
       </c>
-      <c r="D2" s="116" t="s">
+      <c r="D2" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="116" t="s">
+      <c r="M2" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="104">
+      <c r="N2" s="99">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="D3" s="116" t="s">
+      <c r="D3" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="116" t="s">
+      <c r="J3" s="131" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="D4" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="116" t="s">
+      <c r="J4" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="116" t="s">
+      <c r="M4" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="102">
+      <c r="N4" s="97">
         <f>N1*N2</f>
         <v>38.781627930666666</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="131" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="F5" s="117"/>
-      <c r="J5" s="116" t="s">
+      <c r="F5" s="106"/>
+      <c r="J5" s="131" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="131" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="67" t="s">
@@ -6692,7 +6695,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="131" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="67" t="s">
@@ -6700,700 +6703,700 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="109" t="s">
+      <c r="C9" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="109" t="s">
+      <c r="D9" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="109" t="s">
+      <c r="E9" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="109" t="s">
+      <c r="F9" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="109" t="s">
+      <c r="G9" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="109" t="s">
+      <c r="H9" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="109" t="s">
+      <c r="I9" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="109" t="s">
+      <c r="J9" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="109" t="s">
+      <c r="K9" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="109" t="s">
+      <c r="L9" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="109" t="s">
+      <c r="M9" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="109" t="s">
+      <c r="N9" s="133" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="72">
+      <c r="A10" s="70">
         <v>10</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="70" t="s">
         <v>182</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="70" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="71">
         <v>4.2</v>
       </c>
-      <c r="E10" s="72">
+      <c r="E10" s="70">
         <v>233</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="72">
+      <c r="G10" s="70">
         <v>276</v>
       </c>
-      <c r="H10" s="95" t="s">
+      <c r="H10" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="97" t="s">
+      <c r="I10" s="93" t="s">
         <v>185</v>
       </c>
-      <c r="J10" s="114">
+      <c r="J10" s="104">
         <f>0.233*0.276</f>
         <v>6.4308000000000004E-2</v>
       </c>
-      <c r="K10" s="113">
+      <c r="K10" s="103">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="L10" s="94">
+      <c r="L10" s="90">
         <v>2712</v>
       </c>
-      <c r="M10" s="94">
+      <c r="M10" s="90">
         <v>1</v>
       </c>
-      <c r="N10" s="71">
+      <c r="N10" s="69">
         <f>IF(J10="",D10*M10,D10*J10*K10*L10*M10)</f>
         <v>1.8312346080000004</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="72">
+      <c r="A11" s="70">
         <v>20</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="70" t="s">
         <v>182</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="70" t="s">
         <v>184</v>
       </c>
-      <c r="D11" s="73">
+      <c r="D11" s="71">
         <v>4.2</v>
       </c>
-      <c r="E11" s="72">
+      <c r="E11" s="70">
         <v>250</v>
       </c>
-      <c r="F11" s="72" t="s">
+      <c r="F11" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="72">
+      <c r="G11" s="70">
         <v>200</v>
       </c>
-      <c r="H11" s="95" t="s">
+      <c r="H11" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="97" t="s">
+      <c r="I11" s="93" t="s">
         <v>183</v>
       </c>
-      <c r="J11" s="114">
+      <c r="J11" s="104">
         <f>0.25*0.2</f>
         <v>0.05</v>
       </c>
-      <c r="K11" s="115">
+      <c r="K11" s="105">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="L11" s="94">
+      <c r="L11" s="90">
         <v>2712</v>
       </c>
-      <c r="M11" s="94">
+      <c r="M11" s="90">
         <v>1</v>
       </c>
-      <c r="N11" s="71">
+      <c r="N11" s="69">
         <f>IF(J11="",D11*M11,D11*J11*K11*L11*M11)</f>
         <v>8.5427999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="72">
+      <c r="A12" s="70">
         <v>30</v>
       </c>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="70" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="72" t="s">
+      <c r="C12" s="70" t="s">
         <v>202</v>
       </c>
-      <c r="D12" s="73">
+      <c r="D12" s="71">
         <v>4.2</v>
       </c>
-      <c r="E12" s="72">
+      <c r="E12" s="70">
         <v>168</v>
       </c>
-      <c r="F12" s="72" t="s">
+      <c r="F12" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="72">
+      <c r="G12" s="70">
         <v>42</v>
       </c>
-      <c r="H12" s="95" t="s">
+      <c r="H12" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="97" t="s">
+      <c r="I12" s="93" t="s">
         <v>205</v>
       </c>
-      <c r="J12" s="114">
+      <c r="J12" s="104">
         <f>0.168*0.042</f>
         <v>7.0560000000000006E-3</v>
       </c>
-      <c r="K12" s="113">
+      <c r="K12" s="103">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="L12" s="94">
+      <c r="L12" s="90">
         <v>2712</v>
       </c>
-      <c r="M12" s="94">
+      <c r="M12" s="90">
         <v>1</v>
       </c>
-      <c r="N12" s="71">
+      <c r="N12" s="69">
         <f>IF(J12="",D12*M12,D12*J12*K12*L12*M12)</f>
         <v>0.20092665600000004</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="72">
+      <c r="A13" s="70">
         <v>40</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="70" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="D13" s="73">
+      <c r="D13" s="71">
         <v>4.2</v>
       </c>
-      <c r="E13" s="72">
+      <c r="E13" s="70">
         <v>50</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="F13" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="72">
+      <c r="G13" s="70">
         <v>30</v>
       </c>
-      <c r="H13" s="95" t="s">
+      <c r="H13" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="97" t="s">
+      <c r="I13" s="93" t="s">
         <v>204</v>
       </c>
-      <c r="J13" s="114">
+      <c r="J13" s="104">
         <f>0.05*0.03</f>
         <v>1.5E-3</v>
       </c>
-      <c r="K13" s="113">
+      <c r="K13" s="103">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="L13" s="94">
+      <c r="L13" s="90">
         <v>2712</v>
       </c>
-      <c r="M13" s="94">
+      <c r="M13" s="90">
         <v>1</v>
       </c>
-      <c r="N13" s="71">
+      <c r="N13" s="69">
         <f>IF(J13="",D13*M13,D13*J13*K13*L13*M13)</f>
         <v>4.2714000000000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="72">
+      <c r="A14" s="70">
         <v>50</v>
       </c>
-      <c r="B14" s="126" t="s">
+      <c r="B14" s="113" t="s">
         <v>214</v>
       </c>
-      <c r="C14" s="127" t="s">
+      <c r="C14" s="114" t="s">
         <v>215</v>
       </c>
-      <c r="D14" s="128">
+      <c r="D14" s="115">
         <v>1.85</v>
       </c>
-      <c r="E14" s="127">
+      <c r="E14" s="114">
         <v>8</v>
       </c>
-      <c r="F14" s="127" t="s">
+      <c r="F14" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="127"/>
-      <c r="H14" s="129"/>
-      <c r="I14" s="130"/>
-      <c r="J14" s="131"/>
-      <c r="K14" s="132"/>
-      <c r="L14" s="133"/>
-      <c r="M14" s="134">
+      <c r="G14" s="114"/>
+      <c r="H14" s="116"/>
+      <c r="I14" s="117"/>
+      <c r="J14" s="118"/>
+      <c r="K14" s="119"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="121">
         <v>1</v>
       </c>
-      <c r="N14" s="135">
+      <c r="N14" s="122">
         <f>IF(J14="",D14*M14,D14*J14*K14*L14*M14)</f>
         <v>1.85</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="M15" s="108" t="s">
+      <c r="M15" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="N15" s="112">
+      <c r="N15" s="134">
         <f>SUM(N10:N12)</f>
         <v>10.574961264000001</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="109" t="s">
+      <c r="C17" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="109" t="s">
+      <c r="D17" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="109" t="s">
+      <c r="E17" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="109" t="s">
+      <c r="F17" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="109" t="s">
+      <c r="G17" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="109" t="s">
+      <c r="H17" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="109" t="s">
+      <c r="I17" s="133" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="72">
+      <c r="A18" s="70">
         <v>10</v>
       </c>
-      <c r="B18" s="111" t="s">
+      <c r="B18" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="77" t="s">
         <v>181</v>
       </c>
-      <c r="D18" s="73">
+      <c r="D18" s="71">
         <v>1.3</v>
       </c>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="72">
+      <c r="F18" s="70">
         <v>1</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="73">
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="71">
         <f>IF('EN 01001'!$H18&lt;&gt;"",'EN 01001'!$D18*'EN 01001'!$F18*'EN 01001'!$H18,'EN 01001'!$D18*'EN 01001'!$F18)</f>
         <v>1.3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="72">
+      <c r="A19" s="70">
         <v>20</v>
       </c>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="77" t="s">
         <v>179</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="77" t="s">
         <v>180</v>
       </c>
-      <c r="D19" s="73">
+      <c r="D19" s="71">
         <v>0.01</v>
       </c>
-      <c r="E19" s="72" t="s">
+      <c r="E19" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="72">
+      <c r="F19" s="70">
         <v>166</v>
       </c>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="71">
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="69">
         <f>IF('EN 01001'!$H19&lt;&gt;"",'EN 01001'!$D19*'EN 01001'!$F19*'EN 01001'!$H19,'EN 01001'!$D19*'EN 01001'!$F19)</f>
         <v>1.6600000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="72">
+      <c r="A20" s="70">
         <v>30</v>
       </c>
-      <c r="B20" s="111" t="s">
+      <c r="B20" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="81" t="s">
+      <c r="C20" s="77" t="s">
         <v>178</v>
       </c>
-      <c r="D20" s="73">
+      <c r="D20" s="71">
         <v>1.3</v>
       </c>
-      <c r="E20" s="72" t="s">
+      <c r="E20" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="72">
+      <c r="F20" s="70">
         <v>1</v>
       </c>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="73">
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="71">
         <f>IF('EN 01001'!$H20&lt;&gt;"",'EN 01001'!$D20*'EN 01001'!$F20*'EN 01001'!$H20,'EN 01001'!$D20*'EN 01001'!$F20)</f>
         <v>1.3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="72">
+      <c r="A21" s="70">
         <v>40</v>
       </c>
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="77" t="s">
         <v>179</v>
       </c>
-      <c r="C21" s="81" t="s">
+      <c r="C21" s="77" t="s">
         <v>178</v>
       </c>
-      <c r="D21" s="73">
+      <c r="D21" s="71">
         <v>0.01</v>
       </c>
-      <c r="E21" s="72" t="s">
+      <c r="E21" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="72">
+      <c r="F21" s="70">
         <v>155</v>
       </c>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="71">
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="69">
         <f>IF('EN 01001'!$H21&lt;&gt;"",'EN 01001'!$D21*'EN 01001'!$F21*'EN 01001'!$H21,'EN 01001'!$D21*'EN 01001'!$F21)</f>
         <v>1.55</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="72">
+      <c r="A22" s="70">
         <v>50</v>
       </c>
-      <c r="B22" s="111" t="s">
+      <c r="B22" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C22" s="81" t="s">
+      <c r="C22" s="77" t="s">
         <v>207</v>
       </c>
-      <c r="D22" s="73">
+      <c r="D22" s="71">
         <v>1.3</v>
       </c>
-      <c r="E22" s="72" t="s">
+      <c r="E22" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="70">
         <v>1</v>
       </c>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="71">
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="69">
         <f>IF('EN 01001'!$H22&lt;&gt;"",'EN 01001'!$D22*'EN 01001'!$F22*'EN 01001'!$H22,'EN 01001'!$D22*'EN 01001'!$F22)</f>
         <v>1.3</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="72">
+      <c r="A23" s="70">
         <v>60</v>
       </c>
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="77" t="s">
         <v>179</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="77" t="s">
         <v>207</v>
       </c>
-      <c r="D23" s="73">
+      <c r="D23" s="71">
         <v>0.01</v>
       </c>
-      <c r="E23" s="72" t="s">
+      <c r="E23" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="72">
+      <c r="F23" s="70">
         <v>42</v>
       </c>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="71">
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="69">
         <f>IF('EN 01001'!$H23&lt;&gt;"",'EN 01001'!$D23*'EN 01001'!$F23*'EN 01001'!$H23,'EN 01001'!$D23*'EN 01001'!$F23)</f>
         <v>0.42</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="72">
+      <c r="A24" s="70">
         <v>70</v>
       </c>
-      <c r="B24" s="111" t="s">
+      <c r="B24" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C24" s="81" t="s">
+      <c r="C24" s="77" t="s">
         <v>208</v>
       </c>
-      <c r="D24" s="73">
+      <c r="D24" s="71">
         <v>1.3</v>
       </c>
-      <c r="E24" s="72" t="s">
+      <c r="E24" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="72">
+      <c r="F24" s="70">
         <v>1</v>
       </c>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="71">
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="69">
         <f>IF('EN 01001'!$H24&lt;&gt;"",'EN 01001'!$D24*'EN 01001'!$F24*'EN 01001'!$H24,'EN 01001'!$D24*'EN 01001'!$F24)</f>
         <v>1.3</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="72">
+      <c r="A25" s="70">
         <v>80</v>
       </c>
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="77" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="81" t="s">
+      <c r="C25" s="77" t="s">
         <v>208</v>
       </c>
-      <c r="D25" s="73">
+      <c r="D25" s="71">
         <v>0.01</v>
       </c>
-      <c r="E25" s="72" t="s">
+      <c r="E25" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="72">
+      <c r="F25" s="70">
         <v>16</v>
       </c>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="71">
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="69">
         <f>IF('EN 01001'!$H25&lt;&gt;"",'EN 01001'!$D25*'EN 01001'!$F25*'EN 01001'!$H25,'EN 01001'!$D25*'EN 01001'!$F25)</f>
         <v>0.16</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="72">
+      <c r="A26" s="70">
         <v>90</v>
       </c>
-      <c r="B26" s="81" t="s">
+      <c r="B26" s="77" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="81" t="s">
+      <c r="C26" s="77" t="s">
         <v>206</v>
       </c>
-      <c r="D26" s="73">
+      <c r="D26" s="71">
         <v>0.25</v>
       </c>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="72">
+      <c r="F26" s="70">
         <v>4</v>
       </c>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="71">
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="69">
         <f>IF('EN 01001'!$H26&lt;&gt;"",'EN 01001'!$D26*'EN 01001'!$F26*'EN 01001'!$H26,'EN 01001'!$D26*'EN 01001'!$F26)</f>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="72">
+      <c r="A27" s="70">
         <v>100</v>
       </c>
-      <c r="B27" s="111" t="s">
+      <c r="B27" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="77" t="s">
         <v>210</v>
       </c>
-      <c r="D27" s="73">
+      <c r="D27" s="71">
         <v>1.3</v>
       </c>
-      <c r="E27" s="72" t="s">
+      <c r="E27" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="72">
+      <c r="F27" s="70">
         <v>1</v>
       </c>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="71">
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="69">
         <f>IF('EN 01001'!$H27&lt;&gt;"",'EN 01001'!$D27*'EN 01001'!$F27*'EN 01001'!$H27,'EN 01001'!$D27*'EN 01001'!$F27)</f>
         <v>1.3</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="72">
+      <c r="A28" s="70">
         <v>110</v>
       </c>
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="77" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="81" t="s">
+      <c r="C28" s="77" t="s">
         <v>209</v>
       </c>
-      <c r="D28" s="73">
+      <c r="D28" s="71">
         <v>0.35</v>
       </c>
-      <c r="E28" s="72" t="s">
+      <c r="E28" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="72">
+      <c r="F28" s="70">
         <v>1</v>
       </c>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="71">
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="69">
         <f>IF('EN 01001'!$H28&lt;&gt;"",'EN 01001'!$D28*'EN 01001'!$F28*'EN 01001'!$H28,'EN 01001'!$D28*'EN 01001'!$F28)</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="72">
+      <c r="A29" s="70">
         <v>120</v>
       </c>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="77" t="s">
         <v>159</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="77" t="s">
         <v>216</v>
       </c>
-      <c r="D29" s="73">
+      <c r="D29" s="71">
         <v>0.15</v>
       </c>
-      <c r="E29" s="72" t="s">
+      <c r="E29" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="72">
+      <c r="F29" s="70">
         <v>96</v>
       </c>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="71">
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="69">
         <f>IF('EN 01001'!$H29&lt;&gt;"",'EN 01001'!$D29*'EN 01001'!$F29*'EN 01001'!$H29,'EN 01001'!$D29*'EN 01001'!$F29)</f>
         <v>14.399999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H30" s="108" t="s">
+      <c r="H30" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="I30" s="110">
+      <c r="I30" s="136">
         <f>SUM(I18:I29)</f>
         <v>26.04</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H31" s="78"/>
-      <c r="I31" s="77"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="74"/>
     </row>
     <row r="32" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="109" t="s">
+      <c r="A32" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="109" t="s">
+      <c r="B32" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="109" t="s">
+      <c r="C32" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="109" t="s">
+      <c r="D32" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="109" t="s">
+      <c r="E32" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="109" t="s">
+      <c r="F32" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="109" t="s">
+      <c r="G32" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="109" t="s">
+      <c r="H32" s="133" t="s">
         <v>46</v>
       </c>
-      <c r="I32" s="109" t="s">
+      <c r="I32" s="133" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="72">
+      <c r="A33" s="70">
         <v>10</v>
       </c>
-      <c r="B33" s="72" t="s">
+      <c r="B33" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="C33" s="72" t="s">
+      <c r="C33" s="70" t="s">
         <v>173</v>
       </c>
-      <c r="D33" s="73">
+      <c r="D33" s="71">
         <v>500</v>
       </c>
-      <c r="E33" s="72" t="s">
+      <c r="E33" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="72">
+      <c r="F33" s="70">
         <v>13</v>
       </c>
-      <c r="G33" s="72">
+      <c r="G33" s="70">
         <v>3000</v>
       </c>
-      <c r="H33" s="72">
+      <c r="H33" s="70">
         <v>1</v>
       </c>
-      <c r="I33" s="73">
+      <c r="I33" s="71">
         <f>IF('EN 01001'!$G33&lt;&gt;"",D33*F33/G33*H33,"")</f>
         <v>2.1666666666666665</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H34" s="108" t="s">
+      <c r="H34" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="107">
+      <c r="I34" s="137">
         <f>SUM(I33:I33)</f>
         <v>2.1666666666666665</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H35" s="78"/>
-      <c r="I35" s="77"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="74"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7413,13 +7416,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFCCFFCC"/>
+    <tabColor rgb="FFC4D79B"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="49" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7451,98 +7454,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="101" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="118" t="s">
+      <c r="J1" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="105">
+      <c r="K1" s="100">
         <v>81</v>
       </c>
-      <c r="M1" s="116" t="s">
+      <c r="M1" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="102">
+      <c r="N1" s="97">
         <f>N11+I16</f>
         <v>1.4174720000000001</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="131" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="67" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="D2" s="120" t="s">
+      <c r="D2" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="116" t="s">
+      <c r="M2" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="104">
+      <c r="N2" s="99">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="D3" s="116" t="s">
+      <c r="D3" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="116" t="s">
+      <c r="J3" s="131" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="98" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="D4" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="116" t="s">
+      <c r="J4" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="116" t="s">
+      <c r="M4" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="102">
+      <c r="N4" s="97">
         <f>N1*N2</f>
         <v>2.8349440000000001</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="131" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="F5" s="117"/>
-      <c r="J5" s="116" t="s">
+      <c r="F5" s="106"/>
+      <c r="J5" s="131" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="131" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="67" t="s">
@@ -7550,7 +7553,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="131" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="67" t="s">
@@ -7558,193 +7561,193 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="109" t="s">
+      <c r="C9" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="109" t="s">
+      <c r="D9" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="109" t="s">
+      <c r="E9" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="109" t="s">
+      <c r="F9" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="109" t="s">
+      <c r="G9" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="109" t="s">
+      <c r="H9" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="109" t="s">
+      <c r="I9" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="109" t="s">
+      <c r="J9" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="109" t="s">
+      <c r="K9" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="109" t="s">
+      <c r="L9" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="109" t="s">
+      <c r="M9" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="109" t="s">
+      <c r="N9" s="133" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="72">
+      <c r="A10" s="70">
         <v>10</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="70" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="73">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71">
         <v>2.25</v>
       </c>
-      <c r="E10" s="93">
+      <c r="E10" s="89">
         <f>J10*K10*L10</f>
         <v>9.0431999999999998E-2</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="70" t="s">
         <v>192</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="97" t="s">
+      <c r="G10" s="70"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="93" t="s">
         <v>211</v>
       </c>
-      <c r="J10" s="114">
+      <c r="J10" s="104">
         <f>60*32/1000000</f>
         <v>1.92E-3</v>
       </c>
-      <c r="K10" s="115">
+      <c r="K10" s="105">
         <f>6/1000</f>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L10" s="94">
+      <c r="L10" s="90">
         <v>7850</v>
       </c>
-      <c r="M10" s="94">
+      <c r="M10" s="90">
         <v>1</v>
       </c>
-      <c r="N10" s="71">
+      <c r="N10" s="69">
         <f>IF(J10="",D10*M10,D10*J10*K10*L10*M10)</f>
         <v>0.20347200000000001</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="M11" s="108" t="s">
+      <c r="M11" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="112">
+      <c r="N11" s="134">
         <f>SUM(N10:N10)</f>
         <v>0.20347200000000001</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="109" t="s">
+      <c r="D13" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="109" t="s">
+      <c r="E13" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="109" t="s">
+      <c r="F13" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="109" t="s">
+      <c r="G13" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="109" t="s">
+      <c r="H13" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="109" t="s">
+      <c r="I13" s="133" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="72">
+      <c r="A14" s="70">
         <v>10</v>
       </c>
-      <c r="B14" s="111" t="s">
+      <c r="B14" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="77" t="s">
         <v>191</v>
       </c>
-      <c r="D14" s="73">
+      <c r="D14" s="71">
         <v>1.3</v>
       </c>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="72">
+      <c r="F14" s="70">
         <v>1</v>
       </c>
-      <c r="G14" s="119" t="s">
+      <c r="G14" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="H14" s="72">
+      <c r="H14" s="70">
         <f>1/2</f>
         <v>0.5</v>
       </c>
-      <c r="I14" s="73">
+      <c r="I14" s="71">
         <f>H14*F14*D14</f>
         <v>0.65</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="72">
+      <c r="A15" s="70">
         <v>20</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="77" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="81"/>
-      <c r="D15" s="73">
+      <c r="C15" s="77"/>
+      <c r="D15" s="71">
         <v>0.01</v>
       </c>
-      <c r="E15" s="72" t="s">
+      <c r="E15" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="72">
+      <c r="F15" s="70">
         <v>18.8</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="G15" s="70" t="s">
         <v>189</v>
       </c>
-      <c r="H15" s="72">
+      <c r="H15" s="70">
         <v>3</v>
       </c>
-      <c r="I15" s="73">
+      <c r="I15" s="71">
         <f>H15*F15*D15</f>
         <v>0.56400000000000006</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H16" s="108" t="s">
+      <c r="H16" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="110">
+      <c r="I16" s="136">
         <f>SUM(I14:I15)</f>
         <v>1.214</v>
       </c>
@@ -7767,20 +7770,22 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFCCFFCC"/>
+    <tabColor rgb="FFC4D79B"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="49" zoomScaleNormal="49" zoomScalePageLayoutView="49" workbookViewId="0"/>
+    <sheetView zoomScale="49" zoomScaleNormal="49" zoomScalePageLayoutView="49" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="11.5546875" style="121"/>
+    <col min="1" max="16384" width="11.5546875" style="108"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="109" t="s">
         <v>195</v>
       </c>
     </row>
@@ -7801,13 +7806,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFCCFFCC"/>
+    <tabColor rgb="FFC4D79B"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="49" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="49" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7840,98 +7845,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="101" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="118" t="s">
+      <c r="J1" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="105">
+      <c r="K1" s="100">
         <v>81</v>
       </c>
-      <c r="M1" s="116" t="s">
+      <c r="M1" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="102">
+      <c r="N1" s="97">
         <f>N11+I16</f>
         <v>1.9460502534247164</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="131" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="67" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="123" t="s">
+      <c r="C2" s="110" t="s">
         <v>196</v>
       </c>
-      <c r="D2" s="120" t="s">
+      <c r="D2" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="116" t="s">
+      <c r="M2" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="104">
+      <c r="N2" s="99">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="D3" s="116" t="s">
+      <c r="D3" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="116" t="s">
+      <c r="J3" s="131" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="98" t="s">
         <v>167</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="D4" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="116" t="s">
+      <c r="J4" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="116" t="s">
+      <c r="M4" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="102">
+      <c r="N4" s="97">
         <f>N1*N2</f>
         <v>3.8921005068494328</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="131" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="67" t="s">
         <v>201</v>
       </c>
-      <c r="F5" s="117"/>
-      <c r="J5" s="116" t="s">
+      <c r="F5" s="106"/>
+      <c r="J5" s="131" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="131" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="67" t="s">
@@ -7939,7 +7944,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="131" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="67" t="s">
@@ -7947,87 +7952,87 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="109" t="s">
+      <c r="C9" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="109" t="s">
+      <c r="D9" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="109" t="s">
+      <c r="E9" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="109" t="s">
+      <c r="F9" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="109" t="s">
+      <c r="G9" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="109" t="s">
+      <c r="H9" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="109" t="s">
+      <c r="I9" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="109" t="s">
+      <c r="J9" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="109" t="s">
+      <c r="K9" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="109" t="s">
+      <c r="L9" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="109" t="s">
+      <c r="M9" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="109" t="s">
+      <c r="N9" s="133" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="72">
+      <c r="A10" s="70">
         <v>10</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="70" t="s">
         <v>200</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="73">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71">
         <v>2.25</v>
       </c>
-      <c r="E10" s="93">
+      <c r="E10" s="89">
         <f>J10*K10*L10</f>
         <v>6.3133445966540483E-2</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="70" t="s">
         <v>192</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="97" t="s">
+      <c r="G10" s="70"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="93" t="s">
         <v>212</v>
       </c>
-      <c r="J10" s="114">
+      <c r="J10" s="104">
         <f>PI()*8*8/1000000</f>
         <v>2.0106192982974677E-4</v>
       </c>
-      <c r="K10" s="115">
+      <c r="K10" s="105">
         <f>40/1000</f>
         <v>0.04</v>
       </c>
-      <c r="L10" s="94">
+      <c r="L10" s="90">
         <v>7850</v>
       </c>
-      <c r="M10" s="94">
+      <c r="M10" s="90">
         <v>1</v>
       </c>
-      <c r="N10" s="71">
+      <c r="N10" s="69">
         <f>IF(J10="",D10*M10,D10*J10*K10*L10*M10)</f>
         <v>0.14205025342471611</v>
       </c>
@@ -8036,104 +8041,104 @@
       <c r="J11" s="68" t="s">
         <v>199</v>
       </c>
-      <c r="M11" s="108" t="s">
+      <c r="M11" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="112">
+      <c r="N11" s="134">
         <f>SUM(N10:N10)</f>
         <v>0.14205025342471611</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="109" t="s">
+      <c r="D13" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="109" t="s">
+      <c r="E13" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="109" t="s">
+      <c r="F13" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="109" t="s">
+      <c r="G13" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="109" t="s">
+      <c r="H13" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="109" t="s">
+      <c r="I13" s="133" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="72">
+      <c r="A14" s="70">
         <v>10</v>
       </c>
-      <c r="B14" s="111" t="s">
+      <c r="B14" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="73">
+      <c r="C14" s="77"/>
+      <c r="D14" s="71">
         <v>1.3</v>
       </c>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="72">
+      <c r="F14" s="70">
         <v>1</v>
       </c>
-      <c r="G14" s="119"/>
-      <c r="H14" s="72">
+      <c r="G14" s="107"/>
+      <c r="H14" s="70">
         <v>1</v>
       </c>
-      <c r="I14" s="73">
+      <c r="I14" s="71">
         <f>H14*F14*D14</f>
         <v>1.3</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="72">
+      <c r="A15" s="70">
         <v>20</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="77" t="s">
         <v>213</v>
       </c>
-      <c r="D15" s="73">
+      <c r="D15" s="71">
         <v>0.04</v>
       </c>
-      <c r="E15" s="72" t="s">
+      <c r="E15" s="70" t="s">
         <v>197</v>
       </c>
-      <c r="F15" s="72">
+      <c r="F15" s="70">
         <v>4.2</v>
       </c>
-      <c r="G15" s="119" t="s">
+      <c r="G15" s="107" t="s">
         <v>189</v>
       </c>
-      <c r="H15" s="72">
+      <c r="H15" s="70">
         <v>3</v>
       </c>
-      <c r="I15" s="73">
+      <c r="I15" s="71">
         <f>H15*F15*D15</f>
         <v>0.50400000000000011</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H16" s="108" t="s">
+      <c r="H16" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="110">
+      <c r="I16" s="136">
         <f>SUM(I14:I15)</f>
         <v>1.8040000000000003</v>
       </c>
@@ -8157,20 +8162,22 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFCCFFCC"/>
+    <tabColor rgb="FFC4D79B"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="49" zoomScaleNormal="49" zoomScalePageLayoutView="49" workbookViewId="0"/>
+    <sheetView zoomScale="49" zoomScaleNormal="49" zoomScalePageLayoutView="49" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="11.5546875" style="121"/>
+    <col min="1" max="16384" width="11.5546875" style="108"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="109" t="s">
         <v>201</v>
       </c>
     </row>

</xml_diff>